<commit_message>
🍱 Update workshop fall 2021
</commit_message>
<xml_diff>
--- a/tabellenliebe/05_sortieren_und_filtern.xlsx
+++ b/tabellenliebe/05_sortieren_und_filtern.xlsx
@@ -7,11 +7,11 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Tabellenblatt1!$B$1:$B$1000</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DE59BEFF_71A8_4B9F_B3E7_7990EAE42D11_.wvu.FilterData">Tabellenblatt1!$B$1:$B$1000</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_F68C894A_EE82_4D5E_B2B2_ED3AB4945CA2_.wvu.FilterData">Tabellenblatt1!$B$1:$B$1000</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{DE59BEFF-71A8-4B9F-B3E7-7990EAE42D11}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F68C894A-EE82-4D5E-B2B2-ED3AB4945CA2}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -38307,7 +38307,7 @@
   </sheetData>
   <autoFilter ref="$B$1:$B$1000"/>
   <customSheetViews>
-    <customSheetView guid="{DE59BEFF-71A8-4B9F-B3E7-7990EAE42D11}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F68C894A-EE82-4D5E-B2B2-ED3AB4945CA2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$B$1:$B$1000">
         <filterColumn colId="0">
           <filters>

</xml_diff>